<commit_message>
Adding player APIs and Validation for APIs
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/PlayerData.xlsx
+++ b/src/main/resources/Data/PlayerData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinayaga/Documents/Project/cricket-tournament/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loviaror/Desktop/springBoot/cricket-tournament/src/main/resources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11721C4-8B50-3046-8799-5A121FB71D46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32439E13-9577-204F-8FD2-DE6ED2908DAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{2AF2D2D8-6607-E041-9AF5-EFEE10C87C5D}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15860" xr2:uid="{2AF2D2D8-6607-E041-9AF5-EFEE10C87C5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t>Mahendra Singh Dhoni</t>
   </si>
@@ -106,6 +106,60 @@
   </si>
   <si>
     <t>team</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Usman Khawaja</t>
+  </si>
+  <si>
+    <t>Alex Carey</t>
+  </si>
+  <si>
+    <t>Aaron Finch</t>
+  </si>
+  <si>
+    <t>Tim Paine</t>
+  </si>
+  <si>
+    <t>Shaun Marsh</t>
+  </si>
+  <si>
+    <t>Matthew Wade</t>
+  </si>
+  <si>
+    <t>Marcus Harris</t>
+  </si>
+  <si>
+    <t>Marcus Stoinis</t>
+  </si>
+  <si>
+    <t>D'Arcy Short</t>
+  </si>
+  <si>
+    <t>Pat Cummins</t>
+  </si>
+  <si>
+    <t>David Warner</t>
+  </si>
+  <si>
+    <t>Glenn Maxwell</t>
+  </si>
+  <si>
+    <t>Marnus Labuschagne</t>
+  </si>
+  <si>
+    <t>Ashton Agar</t>
+  </si>
+  <si>
+    <t>Steve Smith</t>
+  </si>
+  <si>
+    <t>Mitchell Stark</t>
+  </si>
+  <si>
+    <t>Jhye Richardson</t>
   </si>
 </sst>
 </file>
@@ -466,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061B4E4B-B1F3-A14F-8EC6-AC9C3FD47CBC}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,6 +777,265 @@
         <v>21</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>